<commit_message>
Fixed a bug and added tests.
</commit_message>
<xml_diff>
--- a/forward/tests/data/test_excel_db.xlsx
+++ b/forward/tests/data/test_excel_db.xlsx
@@ -24,39 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>sample</t>
-  </si>
-  <si>
-    <t>s1</t>
-  </si>
-  <si>
-    <t>s2</t>
-  </si>
-  <si>
-    <t>s3</t>
-  </si>
-  <si>
-    <t>s4</t>
-  </si>
-  <si>
-    <t>s5</t>
-  </si>
-  <si>
-    <t>s6</t>
-  </si>
-  <si>
-    <t>s7</t>
-  </si>
-  <si>
-    <t>s8</t>
-  </si>
-  <si>
-    <t>s9</t>
-  </si>
-  <si>
-    <t>s10</t>
   </si>
   <si>
     <t>qte1</t>
@@ -107,8 +77,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,7 +360,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -402,24 +373,24 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="A2" s="1">
+        <v>1001</v>
       </c>
       <c r="B2">
         <v>101.201551154</v>
@@ -438,8 +409,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
+      <c r="A3" s="1">
+        <v>3141</v>
       </c>
       <c r="B3">
         <v>97.667417760999996</v>
@@ -458,8 +429,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
+      <c r="A4" s="1">
+        <v>1931</v>
       </c>
       <c r="B4">
         <v>92.016172159099995</v>
@@ -478,8 +449,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
+      <c r="A5" s="1">
+        <v>4151</v>
       </c>
       <c r="B5">
         <v>96.338927921000007</v>
@@ -498,8 +469,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
+      <c r="A6" s="1">
+        <v>2314</v>
       </c>
       <c r="B6">
         <v>103.490498196</v>
@@ -518,8 +489,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>6</v>
+      <c r="A7" s="1">
+        <v>7438</v>
       </c>
       <c r="B7">
         <v>93.297875774000005</v>
@@ -538,8 +509,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>7</v>
+      <c r="A8" s="1">
+        <v>9624</v>
       </c>
       <c r="B8">
         <v>101.433581995</v>
@@ -558,8 +529,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>8</v>
+      <c r="A9" s="1">
+        <v>4412</v>
       </c>
       <c r="B9">
         <v>121.32519032</v>
@@ -578,8 +549,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>9</v>
+      <c r="A10" s="1">
+        <v>2315</v>
       </c>
       <c r="B10">
         <v>90.9449933171</v>
@@ -598,8 +569,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>10</v>
+      <c r="A11" s="1">
+        <v>2561</v>
       </c>
       <c r="B11">
         <v>97.150071673699998</v>

</xml_diff>